<commit_message>
[305649] Rename Volume to Ton Cost
</commit_message>
<xml_diff>
--- a/Module.Frontend.TPM/Content/Templates/ActualCOGSTnPreTemplate.xlsx
+++ b/Module.Frontend.TPM/Content/Templates/ActualCOGSTnPreTemplate.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmartCom\TPM\Module.Frontend.TPM\Content\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C89480-B9AF-4E1B-A776-9A69E85AD948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF679C41-362F-4E3E-B5D1-A65EA39AE509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A1C29457-48DB-40CA-8C23-00B9FCB4DECF}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <definedName name="Brand_Techs">Лист3!$A$2:$A$1048576</definedName>
     <definedName name="Clientname">Лист2!$A:$A</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -656,7 +656,7 @@
     <t>Brand Techs</t>
   </si>
   <si>
-    <t>Volume</t>
+    <t>Ton Cost</t>
   </si>
 </sst>
 </file>
@@ -4336,18 +4336,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4509,6 +4509,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF790A51-FD04-4AEC-B993-A28DDCB9C542}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3FEE29B2-6E01-4845-B80D-A902E1773A33}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -4520,14 +4528,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="13f900c0-3409-4945-9ad3-55cdae6b8bba"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF790A51-FD04-4AEC-B993-A28DDCB9C542}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>